<commit_message>
Supp functions partial class
</commit_message>
<xml_diff>
--- a/NyilvWebApi/file0.xlsx
+++ b/NyilvWebApi/file0.xlsx
@@ -30,10 +30,10 @@
     <t>Bér</t>
   </si>
   <si>
-    <t>Iparűzési</t>
+    <t>megjegyzés</t>
   </si>
   <si>
-    <t>megjegyzés</t>
+    <t>Iparűzési adó</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,10 +392,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="B1">
-        <v>111</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -404,15 +404,15 @@
         <v>42064</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -421,15 +421,15 @@
         <v>42065</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -438,15 +438,15 @@
         <v>42066</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -455,15 +455,15 @@
         <v>42067</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>102</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -472,15 +472,15 @@
         <v>42068</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -489,32 +489,32 @@
         <v>42069</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>117</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>42070</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -523,32 +523,32 @@
         <v>42071</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>103</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
         <v>42072</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>103</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -557,15 +557,15 @@
         <v>42073</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>103</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -574,24 +574,24 @@
         <v>42074</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>103</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1">
         <v>42075</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>